<commit_message>
code devison is done success
</commit_message>
<xml_diff>
--- a/datas2.xlsx
+++ b/datas2.xlsx
@@ -25,9 +25,6 @@
     <t>naren kumar</t>
   </si>
   <si>
-    <t>snarenkumar30gmail.com</t>
-  </si>
-  <si>
     <t>aspire pages</t>
   </si>
   <si>
@@ -47,16 +44,27 @@
   </si>
   <si>
     <t>narenempire3162@gmail.com</t>
+  </si>
+  <si>
+    <t>snarenkumar30@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,16 +87,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,7 +405,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,32 +422,32 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,14 +455,17 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>